<commit_message>
first stage complete data
</commit_message>
<xml_diff>
--- a/results/regression_results.xlsx
+++ b/results/regression_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,47 +441,62 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Source_Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Outcome_Var</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Exclude_Touching</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Source_Type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Outcome_Var</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Include_area</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Include_population</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Coefficient</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>CI_lower</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>CI_upper</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>P-value</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>F-statistic</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Include area</t>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>n_observations</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>R-squared</t>
         </is>
       </c>
     </row>
@@ -489,128 +504,164 @@
       <c r="A2" t="n">
         <v>100</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>amount_final</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>2343.161234190635</v>
-      </c>
-      <c r="F2" t="n">
-        <v>966.0343699749826</v>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>num_power_stations</t>
+        </is>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>3720.288098406287</v>
+        <v>1.041202766831799</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0008684666706168059</v>
+        <v>-0.01699108037007502</v>
       </c>
       <c r="I2" t="n">
-        <v>11.14286251744499</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
+        <v>2.099396614033673</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.05378687140079773</v>
+      </c>
+      <c r="K2" t="n">
+        <v>50.27570070516628</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1065</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.12446255893452</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>150</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>amount_final</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>2408.64891147503</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1203.410468513687</v>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>num_power_stations</t>
+        </is>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>3613.887354436373</v>
+        <v>1.345818573717814</v>
       </c>
       <c r="H3" t="n">
-        <v>9.224803048789009e-05</v>
+        <v>0.3504478116466351</v>
       </c>
       <c r="I3" t="n">
-        <v>15.36518248058039</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
+        <v>2.341189335788992</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.008082660657925679</v>
+      </c>
+      <c r="K3" t="n">
+        <v>48.5934357513277</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1479</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.08994452030390987</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>200</v>
       </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>amount_final</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>2451.119895795444</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1312.973841370819</v>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>num_power_stations</t>
+        </is>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>3589.265950220069</v>
+        <v>1.4267694629089</v>
       </c>
       <c r="H4" t="n">
-        <v>2.520476352967699e-05</v>
+        <v>0.4495863445585357</v>
       </c>
       <c r="I4" t="n">
-        <v>17.84041331080799</v>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
+        <v>2.403952581259264</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.004238403492816602</v>
+      </c>
+      <c r="K4" t="n">
+        <v>39.61248866532684</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1672</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.06650714922733092</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>250</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>amount_final</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>2430.394603174582</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1333.035494611073</v>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>num_power_stations</t>
+        </is>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>3527.753711738091</v>
+        <v>1.533055607148542</v>
       </c>
       <c r="H5" t="n">
-        <v>1.472545123895472e-05</v>
+        <v>0.6003052936548631</v>
       </c>
       <c r="I5" t="n">
-        <v>18.86593319100357</v>
-      </c>
-      <c r="J5" t="b">
-        <v>0</v>
+        <v>2.465805920642221</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.001288495079580839</v>
+      </c>
+      <c r="K5" t="n">
+        <v>40.27802394708902</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1853</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.06134225900982593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>